<commit_message>
Se actualizó excel de carteras y regex en flujo para que pueda tener referencia del nombre de cartera
</commit_message>
<xml_diff>
--- a/Carteras.xlsx
+++ b/Carteras.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="90">
   <si>
     <t>SECTOR</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>EFECTIVO SI TARDIA</t>
+  </si>
+  <si>
+    <t>EST_TD</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1239,7 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -2260,7 +2263,9 @@
       <c r="B60" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C60" s="4"/>
+      <c r="C60" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>

</xml_diff>